<commit_message>
Lab 02 Homework finished
</commit_message>
<xml_diff>
--- a/src/algorithms/files/Algorithms.xlsx
+++ b/src/algorithms/files/Algorithms.xlsx
@@ -1,31 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\1.Universidad\ED\ED\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\1.Universidad\ED\ED\src\algorithms\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D1B0C91-E8B2-417E-97F2-8B2EF0C021ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{363700D6-9D6F-4261-A461-9386ED139DF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CCF992AF-B5E5-4430-AB74-059A90E405FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Linear</t>
   </si>
@@ -38,12 +47,24 @@
   <si>
     <t>Logarithmic</t>
   </si>
+  <si>
+    <t>powRec1</t>
+  </si>
+  <si>
+    <t>powRec2</t>
+  </si>
+  <si>
+    <t>powRec3</t>
+  </si>
+  <si>
+    <t>powRec4</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -51,16 +72,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -68,14 +102,52 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Cálculo" xfId="1" builtinId="22"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -105,7 +177,62 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="1"/>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-ES"/>
+              <a:t>Algorithms</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
@@ -144,154 +271,154 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="50"/>
                 <c:pt idx="0">
-                  <c:v>31</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>18</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="8">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>24</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="11">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>30</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="14">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="16">
                   <c:v>36</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>43</c:v>
-                </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="17">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>48</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="23">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>54</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="26">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="28">
                   <c:v>60</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="29">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="31">
                   <c:v>66</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="32">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="34">
                   <c:v>72</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="35">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="37">
                   <c:v>78</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="38">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="40">
                   <c:v>84</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="41">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="43">
                   <c:v>90</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="44">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="46">
                   <c:v>96</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="47">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="49">
                   <c:v>102</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>108</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>114</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>122</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>126</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>132</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>138</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>144</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>150</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>157</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>162</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>168</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>174</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>180</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>186</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>192</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>198</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>205</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>210</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>216</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>222</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>228</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>234</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>241</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>246</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>252</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>258</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>264</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>270</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>276</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>282</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>288</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>294</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>300</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>306</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -299,7 +426,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-29B3-4FA5-839F-1512BFB6348E}"/>
+              <c16:uniqueId val="{00000000-F5C7-4E00-AC92-F0536A73FD45}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -336,154 +463,154 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="50"/>
                 <c:pt idx="0">
-                  <c:v>24</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>54</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>96</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>151</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>216</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>295</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>384</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>486</c:v>
+                  <c:v>162</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>600</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>726</c:v>
+                  <c:v>242</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>864</c:v>
+                  <c:v>288</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1014</c:v>
+                  <c:v>339</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1176</c:v>
+                  <c:v>392</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1351</c:v>
+                  <c:v>450</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1537</c:v>
+                  <c:v>512</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1734</c:v>
+                  <c:v>578</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1946</c:v>
+                  <c:v>648</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2166</c:v>
+                  <c:v>722</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2402</c:v>
+                  <c:v>800</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2648</c:v>
+                  <c:v>882</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2904</c:v>
+                  <c:v>968</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>3180</c:v>
+                  <c:v>1060</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>3460</c:v>
+                  <c:v>1153</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>3757</c:v>
+                  <c:v>1251</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>4063</c:v>
+                  <c:v>1354</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>4379</c:v>
+                  <c:v>1459</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>4709</c:v>
+                  <c:v>1569</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>5051</c:v>
+                  <c:v>1683</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>5405</c:v>
+                  <c:v>1804</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>5768</c:v>
+                  <c:v>1923</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>6151</c:v>
+                  <c:v>2049</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>6541</c:v>
+                  <c:v>2180</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>6945</c:v>
+                  <c:v>2314</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>7356</c:v>
+                  <c:v>2452</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>7780</c:v>
+                  <c:v>2594</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>8224</c:v>
+                  <c:v>2740</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>8675</c:v>
+                  <c:v>2889</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>9133</c:v>
+                  <c:v>3045</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>9613</c:v>
+                  <c:v>3205</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>10101</c:v>
+                  <c:v>3366</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>10597</c:v>
+                  <c:v>3531</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>11108</c:v>
+                  <c:v>3699</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>11627</c:v>
+                  <c:v>3874</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>12165</c:v>
+                  <c:v>4052</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>12713</c:v>
+                  <c:v>4237</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>13264</c:v>
+                  <c:v>4420</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>13837</c:v>
+                  <c:v>4610</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>14411</c:v>
+                  <c:v>4804</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>15012</c:v>
+                  <c:v>5001</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>15620</c:v>
+                  <c:v>5206</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -491,7 +618,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-29B3-4FA5-839F-1512BFB6348E}"/>
+              <c16:uniqueId val="{00000001-F5C7-4E00-AC92-F0536A73FD45}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -528,64 +655,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="50"/>
                 <c:pt idx="0">
-                  <c:v>48</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>162</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>384</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>751</c:v>
+                  <c:v>250</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1296</c:v>
+                  <c:v>432</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2058</c:v>
+                  <c:v>687</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3076</c:v>
+                  <c:v>1024</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4375</c:v>
+                  <c:v>1460</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6005</c:v>
+                  <c:v>2003</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7993</c:v>
+                  <c:v>2663</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10378</c:v>
+                  <c:v>3457</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>13189</c:v>
+                  <c:v>4396</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>16472</c:v>
+                  <c:v>5493</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>20266</c:v>
+                  <c:v>6759</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>24586</c:v>
+                  <c:v>8198</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>29488</c:v>
+                  <c:v>9838</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>35008</c:v>
+                  <c:v>11674</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>41185</c:v>
+                  <c:v>13726</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>48061</c:v>
+                  <c:v>16004</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>55634</c:v>
+                  <c:v>18528</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -593,7 +720,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-29B3-4FA5-839F-1512BFB6348E}"/>
+              <c16:uniqueId val="{00000002-F5C7-4E00-AC92-F0536A73FD45}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -785,7 +912,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-29B3-4FA5-839F-1512BFB6348E}"/>
+              <c16:uniqueId val="{00000003-F5C7-4E00-AC92-F0536A73FD45}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -798,17 +925,16 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1766525615"/>
-        <c:axId val="1766527695"/>
+        <c:axId val="500747248"/>
+        <c:axId val="502577088"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1766525615"/>
+        <c:axId val="500747248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -845,7 +971,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1766527695"/>
+        <c:crossAx val="502577088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -853,7 +979,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1766527695"/>
+        <c:axId val="502577088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -904,7 +1030,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1766525615"/>
+        <c:crossAx val="500747248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -949,6 +1075,13 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
@@ -1544,23 +1677,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>352424</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>23811</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Gráfico 1">
+        <xdr:cNvPr id="3" name="Gráfico 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B0A14319-1464-4A37-8B94-3B6AA2B01DDD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A21F7C2E-7F6B-47A0-88A2-79398B3DEEBB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1582,7 +1715,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1598,7 +1731,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -1610,7 +1743,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -1627,7 +1760,7 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -1657,12 +1790,29 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -1692,6 +1842,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1843,638 +2010,874 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D51"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{038DB7A7-3C35-4A5C-9D58-BFDDEE5A6F77}">
+  <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S33" sqref="S33"/>
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>31</v>
-      </c>
-      <c r="B2">
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1">
+        <v>16</v>
+      </c>
+      <c r="D2" s="1">
         <v>24</v>
       </c>
-      <c r="C2">
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1">
+        <v>18</v>
+      </c>
+      <c r="C3" s="1">
+        <v>54</v>
+      </c>
+      <c r="D3" s="1">
+        <v>12</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1">
+        <v>32</v>
+      </c>
+      <c r="C4" s="1">
+        <v>128</v>
+      </c>
+      <c r="D4" s="1">
+        <v>12</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1">
+        <v>50</v>
+      </c>
+      <c r="C5" s="1">
+        <v>250</v>
+      </c>
+      <c r="D5" s="1">
+        <v>18</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1">
+        <v>72</v>
+      </c>
+      <c r="C6" s="1">
+        <v>432</v>
+      </c>
+      <c r="D6" s="1">
+        <v>18</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1">
+        <v>98</v>
+      </c>
+      <c r="C7" s="1">
+        <v>687</v>
+      </c>
+      <c r="D7" s="1">
+        <v>19</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>16</v>
+      </c>
+      <c r="B8" s="1">
+        <v>128</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1024</v>
+      </c>
+      <c r="D8" s="1">
+        <v>18</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>18</v>
+      </c>
+      <c r="B9" s="1">
+        <v>162</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1460</v>
+      </c>
+      <c r="D9" s="1">
+        <v>24</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>20</v>
+      </c>
+      <c r="B10" s="1">
+        <v>200</v>
+      </c>
+      <c r="C10" s="1">
+        <v>2003</v>
+      </c>
+      <c r="D10" s="1">
+        <v>25</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>22</v>
+      </c>
+      <c r="B11" s="1">
+        <v>242</v>
+      </c>
+      <c r="C11" s="1">
+        <v>2663</v>
+      </c>
+      <c r="D11" s="1">
+        <v>24</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>24</v>
+      </c>
+      <c r="B12" s="1">
+        <v>288</v>
+      </c>
+      <c r="C12" s="1">
+        <v>3457</v>
+      </c>
+      <c r="D12" s="1">
+        <v>24</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>26</v>
+      </c>
+      <c r="B13" s="1">
+        <v>339</v>
+      </c>
+      <c r="C13" s="1">
+        <v>4396</v>
+      </c>
+      <c r="D13" s="1">
+        <v>24</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>28</v>
+      </c>
+      <c r="B14" s="1">
+        <v>392</v>
+      </c>
+      <c r="C14" s="1">
+        <v>5493</v>
+      </c>
+      <c r="D14" s="1">
+        <v>24</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>30</v>
+      </c>
+      <c r="B15" s="1">
+        <v>450</v>
+      </c>
+      <c r="C15" s="1">
+        <v>6759</v>
+      </c>
+      <c r="D15" s="1">
+        <v>24</v>
+      </c>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>32</v>
+      </c>
+      <c r="B16" s="1">
+        <v>512</v>
+      </c>
+      <c r="C16" s="1">
+        <v>8198</v>
+      </c>
+      <c r="D16" s="1">
+        <v>24</v>
+      </c>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>34</v>
+      </c>
+      <c r="B17" s="1">
+        <v>578</v>
+      </c>
+      <c r="C17" s="1">
+        <v>9838</v>
+      </c>
+      <c r="D17" s="1">
+        <v>30</v>
+      </c>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>36</v>
+      </c>
+      <c r="B18" s="1">
+        <v>648</v>
+      </c>
+      <c r="C18" s="1">
+        <v>11674</v>
+      </c>
+      <c r="D18" s="1">
+        <v>30</v>
+      </c>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>38</v>
+      </c>
+      <c r="B19" s="1">
+        <v>722</v>
+      </c>
+      <c r="C19" s="1">
+        <v>13726</v>
+      </c>
+      <c r="D19" s="1">
+        <v>30</v>
+      </c>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>40</v>
+      </c>
+      <c r="B20" s="1">
+        <v>800</v>
+      </c>
+      <c r="C20" s="1">
+        <v>16004</v>
+      </c>
+      <c r="D20" s="1">
+        <v>30</v>
+      </c>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>42</v>
+      </c>
+      <c r="B21" s="1">
+        <v>882</v>
+      </c>
+      <c r="C21" s="1">
+        <v>18528</v>
+      </c>
+      <c r="D21" s="1">
+        <v>30</v>
+      </c>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>44</v>
+      </c>
+      <c r="B22" s="1">
+        <v>968</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1">
+        <v>30</v>
+      </c>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>46</v>
+      </c>
+      <c r="B23" s="1">
+        <v>1060</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1">
+        <v>30</v>
+      </c>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
         <v>48</v>
       </c>
-      <c r="D2">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>18</v>
-      </c>
-      <c r="B3">
+      <c r="B24" s="1">
+        <v>1153</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1">
+        <v>30</v>
+      </c>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>50</v>
+      </c>
+      <c r="B25" s="1">
+        <v>1251</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1">
+        <v>30</v>
+      </c>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>52</v>
+      </c>
+      <c r="B26" s="1">
+        <v>1354</v>
+      </c>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1">
+        <v>30</v>
+      </c>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
         <v>54</v>
       </c>
-      <c r="C3">
-        <v>162</v>
-      </c>
-      <c r="D3">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>24</v>
-      </c>
-      <c r="B4">
+      <c r="B27" s="1">
+        <v>1459</v>
+      </c>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1">
+        <v>30</v>
+      </c>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>56</v>
+      </c>
+      <c r="B28" s="1">
+        <v>1569</v>
+      </c>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1">
+        <v>30</v>
+      </c>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>58</v>
+      </c>
+      <c r="B29" s="1">
+        <v>1683</v>
+      </c>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1">
+        <v>30</v>
+      </c>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>60</v>
+      </c>
+      <c r="B30" s="1">
+        <v>1804</v>
+      </c>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1">
+        <v>30</v>
+      </c>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>62</v>
+      </c>
+      <c r="B31" s="1">
+        <v>1923</v>
+      </c>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1">
+        <v>30</v>
+      </c>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>64</v>
+      </c>
+      <c r="B32" s="1">
+        <v>2049</v>
+      </c>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1">
+        <v>30</v>
+      </c>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>66</v>
+      </c>
+      <c r="B33" s="1">
+        <v>2180</v>
+      </c>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1">
+        <v>36</v>
+      </c>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>68</v>
+      </c>
+      <c r="B34" s="1">
+        <v>2314</v>
+      </c>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1">
+        <v>36</v>
+      </c>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>70</v>
+      </c>
+      <c r="B35" s="1">
+        <v>2452</v>
+      </c>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1">
+        <v>37</v>
+      </c>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>72</v>
+      </c>
+      <c r="B36" s="1">
+        <v>2594</v>
+      </c>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1">
+        <v>37</v>
+      </c>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>74</v>
+      </c>
+      <c r="B37" s="1">
+        <v>2740</v>
+      </c>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1">
+        <v>36</v>
+      </c>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>76</v>
+      </c>
+      <c r="B38" s="1">
+        <v>2889</v>
+      </c>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1">
+        <v>36</v>
+      </c>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>78</v>
+      </c>
+      <c r="B39" s="1">
+        <v>3045</v>
+      </c>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1">
+        <v>36</v>
+      </c>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>80</v>
+      </c>
+      <c r="B40" s="1">
+        <v>3205</v>
+      </c>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1">
+        <v>36</v>
+      </c>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>82</v>
+      </c>
+      <c r="B41" s="1">
+        <v>3366</v>
+      </c>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1">
+        <v>36</v>
+      </c>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>84</v>
+      </c>
+      <c r="B42" s="1">
+        <v>3531</v>
+      </c>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1">
+        <v>36</v>
+      </c>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>86</v>
+      </c>
+      <c r="B43" s="1">
+        <v>3699</v>
+      </c>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1">
+        <v>36</v>
+      </c>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>88</v>
+      </c>
+      <c r="B44" s="1">
+        <v>3874</v>
+      </c>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1">
+        <v>36</v>
+      </c>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>90</v>
+      </c>
+      <c r="B45" s="1">
+        <v>4052</v>
+      </c>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1">
+        <v>36</v>
+      </c>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>92</v>
+      </c>
+      <c r="B46" s="1">
+        <v>4237</v>
+      </c>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1">
+        <v>36</v>
+      </c>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>94</v>
+      </c>
+      <c r="B47" s="1">
+        <v>4420</v>
+      </c>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1">
+        <v>36</v>
+      </c>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
         <v>96</v>
       </c>
-      <c r="C4">
-        <v>384</v>
-      </c>
-      <c r="D4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>30</v>
-      </c>
-      <c r="B5">
-        <v>151</v>
-      </c>
-      <c r="C5">
-        <v>751</v>
-      </c>
-      <c r="D5">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="B48" s="1">
+        <v>4610</v>
+      </c>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1">
         <v>36</v>
       </c>
-      <c r="B6">
-        <v>216</v>
-      </c>
-      <c r="C6">
-        <v>1296</v>
-      </c>
-      <c r="D6">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>43</v>
-      </c>
-      <c r="B7">
-        <v>295</v>
-      </c>
-      <c r="C7">
-        <v>2058</v>
-      </c>
-      <c r="D7">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>48</v>
-      </c>
-      <c r="B8">
-        <v>384</v>
-      </c>
-      <c r="C8">
-        <v>3076</v>
-      </c>
-      <c r="D8">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>54</v>
-      </c>
-      <c r="B9">
-        <v>486</v>
-      </c>
-      <c r="C9">
-        <v>4375</v>
-      </c>
-      <c r="D9">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>60</v>
-      </c>
-      <c r="B10">
-        <v>600</v>
-      </c>
-      <c r="C10">
-        <v>6005</v>
-      </c>
-      <c r="D10">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>66</v>
-      </c>
-      <c r="B11">
-        <v>726</v>
-      </c>
-      <c r="C11">
-        <v>7993</v>
-      </c>
-      <c r="D11">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>72</v>
-      </c>
-      <c r="B12">
-        <v>864</v>
-      </c>
-      <c r="C12">
-        <v>10378</v>
-      </c>
-      <c r="D12">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>78</v>
-      </c>
-      <c r="B13">
-        <v>1014</v>
-      </c>
-      <c r="C13">
-        <v>13189</v>
-      </c>
-      <c r="D13">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>84</v>
-      </c>
-      <c r="B14">
-        <v>1176</v>
-      </c>
-      <c r="C14">
-        <v>16472</v>
-      </c>
-      <c r="D14">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>90</v>
-      </c>
-      <c r="B15">
-        <v>1351</v>
-      </c>
-      <c r="C15">
-        <v>20266</v>
-      </c>
-      <c r="D15">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>96</v>
-      </c>
-      <c r="B16">
-        <v>1537</v>
-      </c>
-      <c r="C16">
-        <v>24586</v>
-      </c>
-      <c r="D16">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+      <c r="H48" s="1"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>98</v>
+      </c>
+      <c r="B49" s="1">
+        <v>4804</v>
+      </c>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1">
+        <v>36</v>
+      </c>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+      <c r="H49" s="1"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>100</v>
+      </c>
+      <c r="B50" s="1">
+        <v>5001</v>
+      </c>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1">
+        <v>36</v>
+      </c>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
+      <c r="H50" s="1"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51">
         <v>102</v>
       </c>
-      <c r="B17">
-        <v>1734</v>
-      </c>
-      <c r="C17">
-        <v>29488</v>
-      </c>
-      <c r="D17">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>108</v>
-      </c>
-      <c r="B18">
-        <v>1946</v>
-      </c>
-      <c r="C18">
-        <v>35008</v>
-      </c>
-      <c r="D18">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>114</v>
-      </c>
-      <c r="B19">
-        <v>2166</v>
-      </c>
-      <c r="C19">
-        <v>41185</v>
-      </c>
-      <c r="D19">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>122</v>
-      </c>
-      <c r="B20">
-        <v>2402</v>
-      </c>
-      <c r="C20">
-        <v>48061</v>
-      </c>
-      <c r="D20">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>126</v>
-      </c>
-      <c r="B21">
-        <v>2648</v>
-      </c>
-      <c r="C21">
-        <v>55634</v>
-      </c>
-      <c r="D21">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>132</v>
-      </c>
-      <c r="B22">
-        <v>2904</v>
-      </c>
-      <c r="D22">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>138</v>
-      </c>
-      <c r="B23">
-        <v>3180</v>
-      </c>
-      <c r="D23">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>144</v>
-      </c>
-      <c r="B24">
-        <v>3460</v>
-      </c>
-      <c r="D24">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>150</v>
-      </c>
-      <c r="B25">
-        <v>3757</v>
-      </c>
-      <c r="D25">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>157</v>
-      </c>
-      <c r="B26">
-        <v>4063</v>
-      </c>
-      <c r="D26">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>162</v>
-      </c>
-      <c r="B27">
-        <v>4379</v>
-      </c>
-      <c r="D27">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>168</v>
-      </c>
-      <c r="B28">
-        <v>4709</v>
-      </c>
-      <c r="D28">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>174</v>
-      </c>
-      <c r="B29">
-        <v>5051</v>
-      </c>
-      <c r="D29">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>180</v>
-      </c>
-      <c r="B30">
-        <v>5405</v>
-      </c>
-      <c r="D30">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>186</v>
-      </c>
-      <c r="B31">
-        <v>5768</v>
-      </c>
-      <c r="D31">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>192</v>
-      </c>
-      <c r="B32">
-        <v>6151</v>
-      </c>
-      <c r="D32">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>198</v>
-      </c>
-      <c r="B33">
-        <v>6541</v>
-      </c>
-      <c r="D33">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>205</v>
-      </c>
-      <c r="B34">
-        <v>6945</v>
-      </c>
-      <c r="D34">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>210</v>
-      </c>
-      <c r="B35">
-        <v>7356</v>
-      </c>
-      <c r="D35">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>216</v>
-      </c>
-      <c r="B36">
-        <v>7780</v>
-      </c>
-      <c r="D36">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>222</v>
-      </c>
-      <c r="B37">
-        <v>8224</v>
-      </c>
-      <c r="D37">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>228</v>
-      </c>
-      <c r="B38">
-        <v>8675</v>
-      </c>
-      <c r="D38">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>234</v>
-      </c>
-      <c r="B39">
-        <v>9133</v>
-      </c>
-      <c r="D39">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>241</v>
-      </c>
-      <c r="B40">
-        <v>9613</v>
-      </c>
-      <c r="D40">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>246</v>
-      </c>
-      <c r="B41">
-        <v>10101</v>
-      </c>
-      <c r="D41">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>252</v>
-      </c>
-      <c r="B42">
-        <v>10597</v>
-      </c>
-      <c r="D42">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>258</v>
-      </c>
-      <c r="B43">
-        <v>11108</v>
-      </c>
-      <c r="D43">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>264</v>
-      </c>
-      <c r="B44">
-        <v>11627</v>
-      </c>
-      <c r="D44">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>270</v>
-      </c>
-      <c r="B45">
-        <v>12165</v>
-      </c>
-      <c r="D45">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>276</v>
-      </c>
-      <c r="B46">
-        <v>12713</v>
-      </c>
-      <c r="D46">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>282</v>
-      </c>
-      <c r="B47">
-        <v>13264</v>
-      </c>
-      <c r="D47">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>288</v>
-      </c>
-      <c r="B48">
-        <v>13837</v>
-      </c>
-      <c r="D48">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>294</v>
-      </c>
-      <c r="B49">
-        <v>14411</v>
-      </c>
-      <c r="D49">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>300</v>
-      </c>
-      <c r="B50">
-        <v>15012</v>
-      </c>
-      <c r="D50">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <v>306</v>
-      </c>
       <c r="B51">
-        <v>15620</v>
+        <v>5206</v>
       </c>
       <c r="D51">
         <v>36</v>

</xml_diff>